<commit_message>
small tweak to spreadsheet
</commit_message>
<xml_diff>
--- a/pokemon_sheets_vis/pokemon_sheets_vis.xlsx
+++ b/pokemon_sheets_vis/pokemon_sheets_vis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="934">
   <si>
     <t>name</t>
   </si>
@@ -2806,6 +2806,15 @@
   </si>
   <si>
     <t>AVERAGE of stat total</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Top 3</t>
+  </si>
+  <si>
+    <t>Bottom 3</t>
   </si>
   <si>
     <t>COUNTA of type</t>
@@ -2841,7 +2850,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2854,6 +2863,18 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -2861,7 +2882,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2875,6 +2896,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3026,11 +3049,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1939088559"/>
-        <c:axId val="1741388583"/>
+        <c:axId val="9847925"/>
+        <c:axId val="1796716175"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1939088559"/>
+        <c:axId val="9847925"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3082,10 +3105,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1741388583"/>
+        <c:crossAx val="1796716175"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1741388583"/>
+        <c:axId val="1796716175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,7 +3172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1939088559"/>
+        <c:crossAx val="9847925"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3266,11 +3289,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="140586762"/>
-        <c:axId val="1293732277"/>
+        <c:axId val="1867504739"/>
+        <c:axId val="429444861"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140586762"/>
+        <c:axId val="1867504739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3322,10 +3345,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1293732277"/>
+        <c:crossAx val="429444861"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1293732277"/>
+        <c:axId val="429444861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3389,7 +3412,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140586762"/>
+        <c:crossAx val="1867504739"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3506,11 +3529,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1916522585"/>
-        <c:axId val="65950708"/>
+        <c:axId val="891037727"/>
+        <c:axId val="1681920568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1916522585"/>
+        <c:axId val="891037727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3562,10 +3585,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65950708"/>
+        <c:crossAx val="1681920568"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65950708"/>
+        <c:axId val="1681920568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3640,7 +3663,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916522585"/>
+        <c:crossAx val="891037727"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -69725,7 +69748,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="10.25"/>
-    <col customWidth="1" min="2" max="2" width="13.13"/>
+    <col customWidth="1" min="2" max="2" width="17.5"/>
     <col customWidth="1" min="3" max="3" width="3.38"/>
     <col customWidth="1" min="4" max="4" width="10.25"/>
     <col customWidth="1" min="5" max="5" width="15.75"/>
@@ -69801,7 +69824,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="11" max="11" width="17.75"/>
+    <col customWidth="1" min="10" max="10" width="7.63"/>
+    <col customWidth="1" min="11" max="11" width="8.25"/>
     <col customWidth="1" min="13" max="13" width="7.63"/>
     <col customWidth="1" min="14" max="14" width="4.5"/>
     <col customWidth="1" min="15" max="15" width="8.5"/>
@@ -69809,6 +69833,23 @@
   <sheetData>
     <row r="2">
       <c r="M2" s="4"/>
+    </row>
+    <row r="32">
+      <c r="J32" s="4" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="J33" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34">
+      <c r="J34" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="K34" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
made small small tweaks to pokemon spreadsheet
</commit_message>
<xml_diff>
--- a/pokemon_sheets_vis/pokemon_sheets_vis.xlsx
+++ b/pokemon_sheets_vis/pokemon_sheets_vis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="931">
   <si>
     <t>name</t>
   </si>
@@ -2806,15 +2806,6 @@
   </si>
   <si>
     <t>AVERAGE of stat total</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>Top 3</t>
-  </si>
-  <si>
-    <t>Bottom 3</t>
   </si>
   <si>
     <t>COUNTA of type</t>
@@ -2850,7 +2841,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2861,18 +2852,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6AA84F"/>
-        <bgColor rgb="FF6AA84F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2890,14 +2869,16 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2963,7 +2944,20 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="CC0000"/>
+                <a:srgbClr val="6AA84F"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="6AA84F"/>
               </a:solidFill>
               <a:ln cmpd="sng">
                 <a:solidFill>
@@ -2987,6 +2981,15 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="CC0000"/>
@@ -2999,7 +3002,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="12"/>
+            <c:idx val="16"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="CC0000"/>
@@ -3012,23 +3015,10 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="14"/>
+            <c:idx val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="6AA84F"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="16"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="6AA84F"/>
+                <a:srgbClr val="CC0000"/>
               </a:solidFill>
               <a:ln cmpd="sng">
                 <a:solidFill>
@@ -3049,11 +3039,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="9847925"/>
-        <c:axId val="1796716175"/>
+        <c:axId val="1511852398"/>
+        <c:axId val="119947567"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="9847925"/>
+        <c:axId val="1511852398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3105,10 +3095,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1796716175"/>
+        <c:crossAx val="119947567"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1796716175"/>
+        <c:axId val="119947567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3172,7 +3162,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9847925"/>
+        <c:crossAx val="1511852398"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3289,11 +3279,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1867504739"/>
-        <c:axId val="429444861"/>
+        <c:axId val="547843104"/>
+        <c:axId val="2102569684"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1867504739"/>
+        <c:axId val="547843104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3345,10 +3335,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="429444861"/>
+        <c:crossAx val="2102569684"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="429444861"/>
+        <c:axId val="2102569684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3412,7 +3402,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1867504739"/>
+        <c:crossAx val="547843104"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3529,11 +3519,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="891037727"/>
-        <c:axId val="1681920568"/>
+        <c:axId val="1404194817"/>
+        <c:axId val="1937916219"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="891037727"/>
+        <c:axId val="1404194817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,10 +3575,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1681920568"/>
+        <c:crossAx val="1937916219"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1681920568"/>
+        <c:axId val="1937916219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,7 +3653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="891037727"/>
+        <c:crossAx val="1404194817"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -13043,28 +13033,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -16064,28 +16063,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -19085,28 +19093,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -22106,28 +22123,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -25127,28 +25153,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -28347,28 +28382,37 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="type" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="type" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="15"/>
-        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="5"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item x="16"/>
-        <item x="2"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="secondary type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -31391,29 +31435,38 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="secondary type" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+    <pivotField name="secondary type" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
       <items>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
         <item x="17"/>
-        <item x="15"/>
-        <item x="14"/>
-        <item x="12"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="13"/>
-        <item x="2"/>
-        <item x="16"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="1"/>
         <item x="18"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="11"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea>
+          <references>
+            <reference field="4294967294">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField name="hp" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -32294,7 +32347,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -69760,35 +69816,135 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>923</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="C2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="C3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="C4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="C5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="C6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="C7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="C10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="C11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="C12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="C13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="C15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="C17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="C18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="C19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20">
+      <c r="C20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
     <row r="22"/>
     <row r="23"/>
     <row r="24"/>
@@ -69832,24 +69988,10 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="M2" s="4"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="32">
-      <c r="J32" s="4" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="J33" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34">
-      <c r="J34" s="1" t="s">
-        <v>931</v>
-      </c>
-      <c r="K34" s="6"/>
+      <c r="J32" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>